<commit_message>
Method added to MCQ called createVehicleQuestion() which creates a question based on the characters of given vehicle.
</commit_message>
<xml_diff>
--- a/Veale's NOC List/Veale's vehicle fleet.xlsx
+++ b/Veale's NOC List/Veale's vehicle fleet.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rowley\git\panopoly\Veale's NOC List\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25605" windowHeight="16065" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -2009,6 +2014,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -2336,18 +2349,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C524"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView tabSelected="1" topLeftCell="A151" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="A158" sqref="A158"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="18" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="18.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="17" style="6" customWidth="1"/>
-    <col min="2" max="2" width="41.1640625" style="2" customWidth="1"/>
-    <col min="3" max="3" width="24.33203125" style="6" customWidth="1"/>
+    <col min="2" max="2" width="41.125" style="2" customWidth="1"/>
+    <col min="3" max="3" width="24.375" style="6" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="27" customHeight="1">
+    <row r="1" spans="1:3" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
@@ -2358,7 +2371,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="21" customHeight="1">
+    <row r="2" spans="1:3" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>508</v>
       </c>
@@ -2369,7 +2382,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="21" customHeight="1">
+    <row r="3" spans="1:3" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>508</v>
       </c>
@@ -2380,7 +2393,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="22" customHeight="1">
+    <row r="4" spans="1:3" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>508</v>
       </c>
@@ -2391,7 +2404,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="21" customHeight="1">
+    <row r="5" spans="1:3" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>508</v>
       </c>
@@ -2402,7 +2415,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="21" customHeight="1">
+    <row r="6" spans="1:3" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>508</v>
       </c>
@@ -2413,7 +2426,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="21" customHeight="1">
+    <row r="7" spans="1:3" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>508</v>
       </c>
@@ -2424,7 +2437,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="21" customHeight="1">
+    <row r="8" spans="1:3" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>508</v>
       </c>
@@ -2435,7 +2448,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="22" customHeight="1">
+    <row r="9" spans="1:3" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>508</v>
       </c>
@@ -2446,7 +2459,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="10" spans="1:3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>508</v>
       </c>
@@ -2457,7 +2470,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="11" spans="1:3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>508</v>
       </c>
@@ -2468,7 +2481,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="12" spans="1:3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>508</v>
       </c>
@@ -2479,7 +2492,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="13" spans="1:3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>508</v>
       </c>
@@ -2490,7 +2503,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="14" spans="1:3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>508</v>
       </c>
@@ -2501,7 +2514,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="15" spans="1:3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>508</v>
       </c>
@@ -2512,7 +2525,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="16" spans="1:3">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>508</v>
       </c>
@@ -2523,7 +2536,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="17" spans="1:3">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>508</v>
       </c>
@@ -2534,7 +2547,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="18" spans="1:3">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>508</v>
       </c>
@@ -2545,7 +2558,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="19" spans="1:3">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>508</v>
       </c>
@@ -2556,7 +2569,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="20" spans="1:3">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>508</v>
       </c>
@@ -2567,7 +2580,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="21" spans="1:3">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>508</v>
       </c>
@@ -2578,7 +2591,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="22" spans="1:3">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>508</v>
       </c>
@@ -2589,7 +2602,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="23" spans="1:3">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>508</v>
       </c>
@@ -2600,7 +2613,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="24" spans="1:3">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>508</v>
       </c>
@@ -2611,7 +2624,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="25" spans="1:3">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>508</v>
       </c>
@@ -2622,7 +2635,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="26" spans="1:3">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>508</v>
       </c>
@@ -2633,7 +2646,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="27" spans="1:3">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>508</v>
       </c>
@@ -2644,7 +2657,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="28" spans="1:3">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>508</v>
       </c>
@@ -2655,7 +2668,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="29" spans="1:3">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>508</v>
       </c>
@@ -2666,7 +2679,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="30" spans="1:3">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>508</v>
       </c>
@@ -2677,7 +2690,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="31" spans="1:3">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>508</v>
       </c>
@@ -2688,7 +2701,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="32" spans="1:3">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>508</v>
       </c>
@@ -2699,7 +2712,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="33" spans="1:3">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
         <v>508</v>
       </c>
@@ -2710,7 +2723,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="34" spans="1:3">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
         <v>508</v>
       </c>
@@ -2721,7 +2734,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="35" spans="1:3">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
         <v>508</v>
       </c>
@@ -2732,7 +2745,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="36" spans="1:3">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
         <v>508</v>
       </c>
@@ -2743,7 +2756,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="37" spans="1:3">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
         <v>508</v>
       </c>
@@ -2754,7 +2767,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="38" spans="1:3">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
         <v>508</v>
       </c>
@@ -2765,7 +2778,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="39" spans="1:3">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
         <v>508</v>
       </c>
@@ -2776,7 +2789,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="40" spans="1:3">
+    <row r="40" spans="1:3" ht="37.5" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
         <v>508</v>
       </c>
@@ -2787,7 +2800,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="41" spans="1:3">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
         <v>508</v>
       </c>
@@ -2798,7 +2811,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="42" spans="1:3">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
         <v>508</v>
       </c>
@@ -2809,7 +2822,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="43" spans="1:3">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
         <v>508</v>
       </c>
@@ -2820,7 +2833,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="44" spans="1:3">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
         <v>508</v>
       </c>
@@ -2831,7 +2844,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="45" spans="1:3">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
         <v>508</v>
       </c>
@@ -2842,7 +2855,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="46" spans="1:3">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
         <v>508</v>
       </c>
@@ -2853,7 +2866,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="47" spans="1:3">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
         <v>508</v>
       </c>
@@ -2864,7 +2877,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="48" spans="1:3">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
         <v>508</v>
       </c>
@@ -2875,7 +2888,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="49" spans="1:3">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
         <v>508</v>
       </c>
@@ -2886,7 +2899,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="50" spans="1:3">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
         <v>508</v>
       </c>
@@ -2897,7 +2910,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="51" spans="1:3">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
         <v>508</v>
       </c>
@@ -2908,7 +2921,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="52" spans="1:3">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
         <v>508</v>
       </c>
@@ -2919,7 +2932,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="53" spans="1:3">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
         <v>508</v>
       </c>
@@ -2930,7 +2943,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="54" spans="1:3">
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
         <v>508</v>
       </c>
@@ -2941,7 +2954,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="55" spans="1:3">
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
         <v>508</v>
       </c>
@@ -2952,7 +2965,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="56" spans="1:3">
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
         <v>508</v>
       </c>
@@ -2963,7 +2976,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="57" spans="1:3">
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
         <v>508</v>
       </c>
@@ -2974,7 +2987,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="58" spans="1:3">
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
         <v>508</v>
       </c>
@@ -2985,7 +2998,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="59" spans="1:3">
+    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
         <v>508</v>
       </c>
@@ -2996,7 +3009,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="60" spans="1:3">
+    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
         <v>508</v>
       </c>
@@ -3007,7 +3020,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="61" spans="1:3" ht="36">
+    <row r="61" spans="1:3" ht="37.5" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
         <v>508</v>
       </c>
@@ -3018,7 +3031,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="62" spans="1:3">
+    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
         <v>508</v>
       </c>
@@ -3029,7 +3042,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="63" spans="1:3" ht="36">
+    <row r="63" spans="1:3" ht="37.5" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="s">
         <v>508</v>
       </c>
@@ -3040,7 +3053,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="64" spans="1:3">
+    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
         <v>508</v>
       </c>
@@ -3051,7 +3064,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="65" spans="1:3">
+    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A65" s="1" t="s">
         <v>508</v>
       </c>
@@ -3062,7 +3075,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="66" spans="1:3">
+    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A66" s="1" t="s">
         <v>508</v>
       </c>
@@ -3073,7 +3086,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="67" spans="1:3">
+    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A67" s="1" t="s">
         <v>508</v>
       </c>
@@ -3084,7 +3097,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="68" spans="1:3">
+    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A68" s="1" t="s">
         <v>508</v>
       </c>
@@ -3095,7 +3108,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="69" spans="1:3">
+    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A69" s="1" t="s">
         <v>508</v>
       </c>
@@ -3106,7 +3119,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="70" spans="1:3">
+    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A70" s="1" t="s">
         <v>508</v>
       </c>
@@ -3117,7 +3130,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="71" spans="1:3">
+    <row r="71" spans="1:3" ht="37.5" x14ac:dyDescent="0.25">
       <c r="A71" s="1" t="s">
         <v>508</v>
       </c>
@@ -3128,7 +3141,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="72" spans="1:3">
+    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A72" s="1" t="s">
         <v>508</v>
       </c>
@@ -3139,7 +3152,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="73" spans="1:3">
+    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A73" s="1" t="s">
         <v>508</v>
       </c>
@@ -3150,7 +3163,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="74" spans="1:3">
+    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A74" s="1" t="s">
         <v>508</v>
       </c>
@@ -3161,7 +3174,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="75" spans="1:3">
+    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A75" s="1" t="s">
         <v>508</v>
       </c>
@@ -3172,7 +3185,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="76" spans="1:3">
+    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A76" s="1" t="s">
         <v>508</v>
       </c>
@@ -3183,7 +3196,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="77" spans="1:3">
+    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A77" s="1" t="s">
         <v>508</v>
       </c>
@@ -3194,7 +3207,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="78" spans="1:3">
+    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A78" s="1" t="s">
         <v>508</v>
       </c>
@@ -3205,7 +3218,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="79" spans="1:3">
+    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A79" s="1" t="s">
         <v>508</v>
       </c>
@@ -3216,7 +3229,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="80" spans="1:3">
+    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A80" s="1" t="s">
         <v>508</v>
       </c>
@@ -3227,7 +3240,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="81" spans="1:3">
+    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A81" s="1" t="s">
         <v>508</v>
       </c>
@@ -3238,7 +3251,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="82" spans="1:3">
+    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A82" s="1" t="s">
         <v>508</v>
       </c>
@@ -3249,7 +3262,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="83" spans="1:3">
+    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A83" s="1" t="s">
         <v>508</v>
       </c>
@@ -3260,7 +3273,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="84" spans="1:3">
+    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A84" s="1" t="s">
         <v>508</v>
       </c>
@@ -3271,7 +3284,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="85" spans="1:3">
+    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A85" s="1" t="s">
         <v>508</v>
       </c>
@@ -3282,7 +3295,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="86" spans="1:3">
+    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A86" s="1" t="s">
         <v>508</v>
       </c>
@@ -3293,7 +3306,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="87" spans="1:3">
+    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A87" s="1" t="s">
         <v>508</v>
       </c>
@@ -3304,7 +3317,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="88" spans="1:3">
+    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A88" s="1" t="s">
         <v>508</v>
       </c>
@@ -3315,7 +3328,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="89" spans="1:3">
+    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A89" s="1" t="s">
         <v>508</v>
       </c>
@@ -3326,7 +3339,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="90" spans="1:3">
+    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A90" s="1" t="s">
         <v>508</v>
       </c>
@@ -3337,7 +3350,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="91" spans="1:3">
+    <row r="91" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A91" s="1" t="s">
         <v>508</v>
       </c>
@@ -3348,7 +3361,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="92" spans="1:3">
+    <row r="92" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A92" s="1" t="s">
         <v>508</v>
       </c>
@@ -3359,7 +3372,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="93" spans="1:3">
+    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A93" s="1" t="s">
         <v>508</v>
       </c>
@@ -3370,7 +3383,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="94" spans="1:3">
+    <row r="94" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A94" s="1" t="s">
         <v>508</v>
       </c>
@@ -3381,7 +3394,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="95" spans="1:3">
+    <row r="95" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A95" s="1" t="s">
         <v>508</v>
       </c>
@@ -3392,7 +3405,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="96" spans="1:3">
+    <row r="96" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A96" s="1" t="s">
         <v>508</v>
       </c>
@@ -3403,7 +3416,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="97" spans="1:3">
+    <row r="97" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A97" s="1" t="s">
         <v>508</v>
       </c>
@@ -3414,7 +3427,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="98" spans="1:3">
+    <row r="98" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A98" s="1" t="s">
         <v>508</v>
       </c>
@@ -3425,7 +3438,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="99" spans="1:3">
+    <row r="99" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A99" s="1" t="s">
         <v>508</v>
       </c>
@@ -3436,7 +3449,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="100" spans="1:3">
+    <row r="100" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A100" s="1" t="s">
         <v>508</v>
       </c>
@@ -3447,7 +3460,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="101" spans="1:3">
+    <row r="101" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A101" s="1" t="s">
         <v>508</v>
       </c>
@@ -3458,7 +3471,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="102" spans="1:3">
+    <row r="102" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A102" s="1" t="s">
         <v>508</v>
       </c>
@@ -3469,7 +3482,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="103" spans="1:3">
+    <row r="103" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A103" s="1" t="s">
         <v>508</v>
       </c>
@@ -3480,7 +3493,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="104" spans="1:3">
+    <row r="104" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A104" s="1" t="s">
         <v>508</v>
       </c>
@@ -3491,7 +3504,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="105" spans="1:3">
+    <row r="105" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A105" s="1" t="s">
         <v>508</v>
       </c>
@@ -3502,7 +3515,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="106" spans="1:3">
+    <row r="106" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A106" s="1" t="s">
         <v>508</v>
       </c>
@@ -3513,7 +3526,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="107" spans="1:3">
+    <row r="107" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A107" s="1" t="s">
         <v>508</v>
       </c>
@@ -3524,7 +3537,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="108" spans="1:3">
+    <row r="108" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A108" s="1" t="s">
         <v>508</v>
       </c>
@@ -3535,7 +3548,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="109" spans="1:3">
+    <row r="109" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A109" s="1" t="s">
         <v>508</v>
       </c>
@@ -3546,7 +3559,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="110" spans="1:3">
+    <row r="110" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A110" s="1" t="s">
         <v>508</v>
       </c>
@@ -3557,7 +3570,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="111" spans="1:3">
+    <row r="111" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A111" s="1" t="s">
         <v>508</v>
       </c>
@@ -3568,7 +3581,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="112" spans="1:3">
+    <row r="112" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A112" s="1" t="s">
         <v>508</v>
       </c>
@@ -3579,7 +3592,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="113" spans="1:3">
+    <row r="113" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A113" s="1" t="s">
         <v>508</v>
       </c>
@@ -3590,7 +3603,7 @@
         <v>522</v>
       </c>
     </row>
-    <row r="114" spans="1:3">
+    <row r="114" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A114" s="1" t="s">
         <v>508</v>
       </c>
@@ -3601,7 +3614,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="115" spans="1:3">
+    <row r="115" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A115" s="1" t="s">
         <v>508</v>
       </c>
@@ -3612,7 +3625,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="116" spans="1:3">
+    <row r="116" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A116" s="1" t="s">
         <v>508</v>
       </c>
@@ -3623,7 +3636,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="117" spans="1:3">
+    <row r="117" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A117" s="1" t="s">
         <v>508</v>
       </c>
@@ -3634,7 +3647,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="118" spans="1:3">
+    <row r="118" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A118" s="1" t="s">
         <v>508</v>
       </c>
@@ -3645,7 +3658,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="119" spans="1:3">
+    <row r="119" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A119" s="1" t="s">
         <v>508</v>
       </c>
@@ -3656,7 +3669,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="120" spans="1:3">
+    <row r="120" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A120" s="1" t="s">
         <v>510</v>
       </c>
@@ -3667,7 +3680,7 @@
         <v>521</v>
       </c>
     </row>
-    <row r="121" spans="1:3">
+    <row r="121" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A121" s="1" t="s">
         <v>510</v>
       </c>
@@ -3678,7 +3691,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="122" spans="1:3">
+    <row r="122" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A122" s="1" t="s">
         <v>510</v>
       </c>
@@ -3689,7 +3702,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="123" spans="1:3">
+    <row r="123" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A123" s="1" t="s">
         <v>510</v>
       </c>
@@ -3700,7 +3713,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="124" spans="1:3">
+    <row r="124" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A124" s="1" t="s">
         <v>510</v>
       </c>
@@ -3711,7 +3724,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="125" spans="1:3">
+    <row r="125" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A125" s="1" t="s">
         <v>510</v>
       </c>
@@ -3722,7 +3735,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="126" spans="1:3">
+    <row r="126" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A126" s="1" t="s">
         <v>510</v>
       </c>
@@ -3733,7 +3746,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="127" spans="1:3">
+    <row r="127" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A127" s="1" t="s">
         <v>509</v>
       </c>
@@ -3744,7 +3757,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="128" spans="1:3">
+    <row r="128" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A128" s="1" t="s">
         <v>510</v>
       </c>
@@ -3755,7 +3768,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="129" spans="1:3">
+    <row r="129" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A129" s="1" t="s">
         <v>510</v>
       </c>
@@ -3766,7 +3779,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="130" spans="1:3">
+    <row r="130" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A130" s="3" t="s">
         <v>510</v>
       </c>
@@ -3777,7 +3790,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="131" spans="1:3">
+    <row r="131" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A131" s="3" t="s">
         <v>510</v>
       </c>
@@ -3788,7 +3801,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="132" spans="1:3">
+    <row r="132" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A132" s="3" t="s">
         <v>510</v>
       </c>
@@ -3799,7 +3812,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="133" spans="1:3">
+    <row r="133" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A133" s="3" t="s">
         <v>510</v>
       </c>
@@ -3810,7 +3823,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="134" spans="1:3">
+    <row r="134" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A134" s="3" t="s">
         <v>510</v>
       </c>
@@ -3821,7 +3834,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="135" spans="1:3">
+    <row r="135" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A135" s="3" t="s">
         <v>510</v>
       </c>
@@ -3832,7 +3845,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="136" spans="1:3">
+    <row r="136" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A136" s="3" t="s">
         <v>510</v>
       </c>
@@ -3843,7 +3856,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="137" spans="1:3">
+    <row r="137" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A137" s="3" t="s">
         <v>510</v>
       </c>
@@ -3854,7 +3867,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="138" spans="1:3">
+    <row r="138" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A138" s="3" t="s">
         <v>510</v>
       </c>
@@ -3865,7 +3878,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="139" spans="1:3">
+    <row r="139" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A139" s="3" t="s">
         <v>510</v>
       </c>
@@ -3876,7 +3889,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="140" spans="1:3">
+    <row r="140" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A140" s="3" t="s">
         <v>510</v>
       </c>
@@ -3887,7 +3900,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="141" spans="1:3">
+    <row r="141" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A141" s="3" t="s">
         <v>510</v>
       </c>
@@ -3898,7 +3911,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="142" spans="1:3">
+    <row r="142" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A142" s="3" t="s">
         <v>510</v>
       </c>
@@ -3909,7 +3922,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="143" spans="1:3">
+    <row r="143" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A143" s="3" t="s">
         <v>510</v>
       </c>
@@ -3920,7 +3933,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="144" spans="1:3">
+    <row r="144" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A144" s="1" t="s">
         <v>508</v>
       </c>
@@ -3931,7 +3944,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="145" spans="1:3">
+    <row r="145" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A145" s="1" t="s">
         <v>509</v>
       </c>
@@ -3942,7 +3955,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="146" spans="1:3">
+    <row r="146" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A146" s="1" t="s">
         <v>508</v>
       </c>
@@ -3953,7 +3966,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="147" spans="1:3">
+    <row r="147" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A147" s="1" t="s">
         <v>508</v>
       </c>
@@ -3964,7 +3977,7 @@
         <v>523</v>
       </c>
     </row>
-    <row r="148" spans="1:3">
+    <row r="148" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A148" s="1" t="s">
         <v>508</v>
       </c>
@@ -3975,7 +3988,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="149" spans="1:3">
+    <row r="149" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A149" s="1" t="s">
         <v>508</v>
       </c>
@@ -3986,7 +3999,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="150" spans="1:3">
+    <row r="150" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A150" s="1" t="s">
         <v>508</v>
       </c>
@@ -3997,7 +4010,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="151" spans="1:3">
+    <row r="151" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A151" s="1" t="s">
         <v>508</v>
       </c>
@@ -4008,7 +4021,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="152" spans="1:3">
+    <row r="152" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A152" s="1" t="s">
         <v>508</v>
       </c>
@@ -4019,7 +4032,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="153" spans="1:3">
+    <row r="153" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A153" s="1" t="s">
         <v>508</v>
       </c>
@@ -4030,7 +4043,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="154" spans="1:3">
+    <row r="154" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A154" s="1" t="s">
         <v>508</v>
       </c>
@@ -4041,7 +4054,7 @@
         <v>524</v>
       </c>
     </row>
-    <row r="155" spans="1:3">
+    <row r="155" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A155" s="1" t="s">
         <v>508</v>
       </c>
@@ -4052,7 +4065,7 @@
         <v>521</v>
       </c>
     </row>
-    <row r="156" spans="1:3">
+    <row r="156" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A156" s="1" t="s">
         <v>508</v>
       </c>
@@ -4063,7 +4076,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="157" spans="1:3">
+    <row r="157" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A157" s="1" t="s">
         <v>508</v>
       </c>
@@ -4074,7 +4087,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="158" spans="1:3">
+    <row r="158" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A158" s="1"/>
       <c r="B158" s="2" t="s">
         <v>43</v>
@@ -4083,7 +4096,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="159" spans="1:3">
+    <row r="159" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A159" s="1" t="s">
         <v>508</v>
       </c>
@@ -4094,7 +4107,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="160" spans="1:3">
+    <row r="160" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A160" s="1" t="s">
         <v>508</v>
       </c>
@@ -4105,7 +4118,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="161" spans="1:3">
+    <row r="161" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A161" s="1" t="s">
         <v>508</v>
       </c>
@@ -4116,7 +4129,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="162" spans="1:3">
+    <row r="162" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A162" s="1" t="s">
         <v>508</v>
       </c>
@@ -4127,7 +4140,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="163" spans="1:3">
+    <row r="163" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A163" s="1" t="s">
         <v>508</v>
       </c>
@@ -4138,7 +4151,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="164" spans="1:3">
+    <row r="164" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A164" s="1" t="s">
         <v>508</v>
       </c>
@@ -4149,7 +4162,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="165" spans="1:3">
+    <row r="165" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A165" s="1" t="s">
         <v>508</v>
       </c>
@@ -4160,7 +4173,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="166" spans="1:3">
+    <row r="166" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A166" s="1" t="s">
         <v>508</v>
       </c>
@@ -4171,7 +4184,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="167" spans="1:3">
+    <row r="167" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A167" s="1" t="s">
         <v>508</v>
       </c>
@@ -4182,7 +4195,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="168" spans="1:3">
+    <row r="168" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A168" s="1" t="s">
         <v>508</v>
       </c>
@@ -4193,7 +4206,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="169" spans="1:3">
+    <row r="169" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A169" s="1" t="s">
         <v>508</v>
       </c>
@@ -4204,7 +4217,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="170" spans="1:3">
+    <row r="170" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A170" s="1" t="s">
         <v>508</v>
       </c>
@@ -4215,7 +4228,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="171" spans="1:3">
+    <row r="171" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A171" s="1" t="s">
         <v>508</v>
       </c>
@@ -4226,7 +4239,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="172" spans="1:3">
+    <row r="172" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A172" s="1" t="s">
         <v>508</v>
       </c>
@@ -4237,7 +4250,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="173" spans="1:3">
+    <row r="173" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A173" s="1" t="s">
         <v>508</v>
       </c>
@@ -4248,7 +4261,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="174" spans="1:3">
+    <row r="174" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A174" s="1" t="s">
         <v>508</v>
       </c>
@@ -4259,7 +4272,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="175" spans="1:3">
+    <row r="175" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A175" s="1" t="s">
         <v>508</v>
       </c>
@@ -4270,7 +4283,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="176" spans="1:3">
+    <row r="176" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A176" s="1" t="s">
         <v>508</v>
       </c>
@@ -4281,7 +4294,7 @@
         <v>521</v>
       </c>
     </row>
-    <row r="177" spans="1:3">
+    <row r="177" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A177" s="1" t="s">
         <v>508</v>
       </c>
@@ -4292,7 +4305,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="178" spans="1:3">
+    <row r="178" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A178" s="1" t="s">
         <v>508</v>
       </c>
@@ -4303,7 +4316,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="179" spans="1:3">
+    <row r="179" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A179" s="1" t="s">
         <v>508</v>
       </c>
@@ -4314,7 +4327,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="180" spans="1:3">
+    <row r="180" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A180" s="1" t="s">
         <v>508</v>
       </c>
@@ -4325,7 +4338,7 @@
         <v>521</v>
       </c>
     </row>
-    <row r="181" spans="1:3">
+    <row r="181" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A181" s="1" t="s">
         <v>508</v>
       </c>
@@ -4336,7 +4349,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="182" spans="1:3">
+    <row r="182" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A182" s="1"/>
       <c r="B182" s="2" t="s">
         <v>451</v>
@@ -4345,7 +4358,7 @@
         <v>521</v>
       </c>
     </row>
-    <row r="183" spans="1:3">
+    <row r="183" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A183" s="1" t="s">
         <v>508</v>
       </c>
@@ -4356,7 +4369,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="184" spans="1:3">
+    <row r="184" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A184" s="1" t="s">
         <v>508</v>
       </c>
@@ -4367,7 +4380,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="185" spans="1:3">
+    <row r="185" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A185" s="1" t="s">
         <v>508</v>
       </c>
@@ -4378,7 +4391,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="186" spans="1:3">
+    <row r="186" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A186" s="1" t="s">
         <v>508</v>
       </c>
@@ -4389,7 +4402,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="187" spans="1:3">
+    <row r="187" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A187" s="1" t="s">
         <v>508</v>
       </c>
@@ -4400,7 +4413,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="188" spans="1:3">
+    <row r="188" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A188" s="1" t="s">
         <v>508</v>
       </c>
@@ -4411,7 +4424,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="189" spans="1:3">
+    <row r="189" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A189" s="1" t="s">
         <v>508</v>
       </c>
@@ -4422,7 +4435,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="190" spans="1:3">
+    <row r="190" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A190" s="1" t="s">
         <v>508</v>
       </c>
@@ -4433,7 +4446,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="191" spans="1:3">
+    <row r="191" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A191" s="1" t="s">
         <v>508</v>
       </c>
@@ -4444,7 +4457,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="192" spans="1:3">
+    <row r="192" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A192" s="1" t="s">
         <v>508</v>
       </c>
@@ -4455,7 +4468,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="193" spans="1:3">
+    <row r="193" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A193" s="1" t="s">
         <v>508</v>
       </c>
@@ -4466,7 +4479,7 @@
         <v>521</v>
       </c>
     </row>
-    <row r="194" spans="1:3">
+    <row r="194" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A194" s="1" t="s">
         <v>508</v>
       </c>
@@ -4477,7 +4490,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="195" spans="1:3">
+    <row r="195" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A195" s="1" t="s">
         <v>508</v>
       </c>
@@ -4488,7 +4501,7 @@
         <v>525</v>
       </c>
     </row>
-    <row r="196" spans="1:3">
+    <row r="196" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A196" s="1" t="s">
         <v>508</v>
       </c>
@@ -4499,7 +4512,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="197" spans="1:3">
+    <row r="197" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A197" s="1" t="s">
         <v>508</v>
       </c>
@@ -4510,7 +4523,7 @@
         <v>523</v>
       </c>
     </row>
-    <row r="198" spans="1:3">
+    <row r="198" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A198" s="1" t="s">
         <v>508</v>
       </c>
@@ -4521,7 +4534,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="199" spans="1:3">
+    <row r="199" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A199" s="1" t="s">
         <v>508</v>
       </c>
@@ -4532,7 +4545,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="200" spans="1:3">
+    <row r="200" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A200" s="1" t="s">
         <v>508</v>
       </c>
@@ -4543,7 +4556,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="201" spans="1:3">
+    <row r="201" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A201" s="1" t="s">
         <v>508</v>
       </c>
@@ -4554,7 +4567,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="202" spans="1:3">
+    <row r="202" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A202" s="1" t="s">
         <v>509</v>
       </c>
@@ -4565,7 +4578,7 @@
         <v>522</v>
       </c>
     </row>
-    <row r="203" spans="1:3">
+    <row r="203" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A203" s="1" t="s">
         <v>508</v>
       </c>
@@ -4576,7 +4589,7 @@
         <v>526</v>
       </c>
     </row>
-    <row r="204" spans="1:3">
+    <row r="204" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A204" s="1" t="s">
         <v>508</v>
       </c>
@@ -4587,7 +4600,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="205" spans="1:3">
+    <row r="205" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A205" s="1" t="s">
         <v>508</v>
       </c>
@@ -4598,7 +4611,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="206" spans="1:3">
+    <row r="206" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A206" s="1" t="s">
         <v>508</v>
       </c>
@@ -4609,7 +4622,7 @@
         <v>527</v>
       </c>
     </row>
-    <row r="207" spans="1:3">
+    <row r="207" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A207" s="1" t="s">
         <v>508</v>
       </c>
@@ -4620,7 +4633,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="208" spans="1:3">
+    <row r="208" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A208" s="1"/>
       <c r="B208" s="2" t="s">
         <v>69</v>
@@ -4629,7 +4642,7 @@
         <v>523</v>
       </c>
     </row>
-    <row r="209" spans="1:3">
+    <row r="209" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A209" s="1" t="s">
         <v>508</v>
       </c>
@@ -4640,7 +4653,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="210" spans="1:3">
+    <row r="210" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A210" s="1" t="s">
         <v>508</v>
       </c>
@@ -4651,7 +4664,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="211" spans="1:3">
+    <row r="211" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A211" s="1" t="s">
         <v>508</v>
       </c>
@@ -4662,7 +4675,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="212" spans="1:3">
+    <row r="212" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A212" s="1" t="s">
         <v>508</v>
       </c>
@@ -4673,7 +4686,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="213" spans="1:3">
+    <row r="213" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A213" s="1" t="s">
         <v>508</v>
       </c>
@@ -4684,7 +4697,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="214" spans="1:3">
+    <row r="214" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A214" s="1" t="s">
         <v>509</v>
       </c>
@@ -4695,7 +4708,7 @@
         <v>528</v>
       </c>
     </row>
-    <row r="215" spans="1:3">
+    <row r="215" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A215" s="1" t="s">
         <v>508</v>
       </c>
@@ -4706,7 +4719,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="216" spans="1:3">
+    <row r="216" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A216" s="1" t="s">
         <v>508</v>
       </c>
@@ -4717,7 +4730,7 @@
         <v>521</v>
       </c>
     </row>
-    <row r="217" spans="1:3">
+    <row r="217" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A217" s="1" t="s">
         <v>508</v>
       </c>
@@ -4728,7 +4741,7 @@
         <v>521</v>
       </c>
     </row>
-    <row r="218" spans="1:3">
+    <row r="218" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A218" s="1" t="s">
         <v>508</v>
       </c>
@@ -4739,7 +4752,7 @@
         <v>529</v>
       </c>
     </row>
-    <row r="219" spans="1:3">
+    <row r="219" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A219" s="1" t="s">
         <v>508</v>
       </c>
@@ -4750,7 +4763,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="220" spans="1:3">
+    <row r="220" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A220" s="1" t="s">
         <v>508</v>
       </c>
@@ -4761,7 +4774,7 @@
         <v>530</v>
       </c>
     </row>
-    <row r="221" spans="1:3">
+    <row r="221" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A221" s="1" t="s">
         <v>510</v>
       </c>
@@ -4772,7 +4785,7 @@
         <v>521</v>
       </c>
     </row>
-    <row r="222" spans="1:3">
+    <row r="222" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A222" s="1" t="s">
         <v>510</v>
       </c>
@@ -4783,7 +4796,7 @@
         <v>521</v>
       </c>
     </row>
-    <row r="223" spans="1:3">
+    <row r="223" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A223" s="1" t="s">
         <v>510</v>
       </c>
@@ -4794,7 +4807,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="224" spans="1:3">
+    <row r="224" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A224" s="1" t="s">
         <v>510</v>
       </c>
@@ -4805,7 +4818,7 @@
         <v>531</v>
       </c>
     </row>
-    <row r="225" spans="1:3">
+    <row r="225" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A225" s="1" t="s">
         <v>508</v>
       </c>
@@ -4816,7 +4829,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="226" spans="1:3">
+    <row r="226" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A226" s="1" t="s">
         <v>508</v>
       </c>
@@ -4827,7 +4840,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="227" spans="1:3">
+    <row r="227" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A227" s="1" t="s">
         <v>508</v>
       </c>
@@ -4838,7 +4851,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="228" spans="1:3">
+    <row r="228" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A228" s="1" t="s">
         <v>508</v>
       </c>
@@ -4849,7 +4862,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="229" spans="1:3">
+    <row r="229" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A229" s="1" t="s">
         <v>508</v>
       </c>
@@ -4860,7 +4873,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="230" spans="1:3">
+    <row r="230" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A230" s="1" t="s">
         <v>508</v>
       </c>
@@ -4871,7 +4884,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="231" spans="1:3">
+    <row r="231" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A231" s="1" t="s">
         <v>508</v>
       </c>
@@ -4882,7 +4895,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="232" spans="1:3">
+    <row r="232" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A232" s="1" t="s">
         <v>508</v>
       </c>
@@ -4893,7 +4906,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="233" spans="1:3">
+    <row r="233" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A233" s="1" t="s">
         <v>508</v>
       </c>
@@ -4904,7 +4917,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="234" spans="1:3">
+    <row r="234" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A234" s="1" t="s">
         <v>508</v>
       </c>
@@ -4915,7 +4928,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="235" spans="1:3">
+    <row r="235" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A235" s="1" t="s">
         <v>508</v>
       </c>
@@ -4926,7 +4939,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="236" spans="1:3">
+    <row r="236" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A236" s="1" t="s">
         <v>508</v>
       </c>
@@ -4937,7 +4950,7 @@
         <v>526</v>
       </c>
     </row>
-    <row r="237" spans="1:3">
+    <row r="237" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A237" s="1"/>
       <c r="B237" s="2" t="s">
         <v>131</v>
@@ -4946,7 +4959,7 @@
         <v>532</v>
       </c>
     </row>
-    <row r="238" spans="1:3">
+    <row r="238" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A238" s="1" t="s">
         <v>508</v>
       </c>
@@ -4957,7 +4970,7 @@
         <v>533</v>
       </c>
     </row>
-    <row r="239" spans="1:3">
+    <row r="239" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A239" s="1" t="s">
         <v>508</v>
       </c>
@@ -4968,7 +4981,7 @@
         <v>534</v>
       </c>
     </row>
-    <row r="240" spans="1:3">
+    <row r="240" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A240" s="1" t="s">
         <v>508</v>
       </c>
@@ -4979,7 +4992,7 @@
         <v>535</v>
       </c>
     </row>
-    <row r="241" spans="1:3">
+    <row r="241" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A241" s="1"/>
       <c r="B241" s="2" t="s">
         <v>405</v>
@@ -4988,7 +5001,7 @@
         <v>536</v>
       </c>
     </row>
-    <row r="242" spans="1:3">
+    <row r="242" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A242" s="1" t="s">
         <v>508</v>
       </c>
@@ -4999,7 +5012,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="243" spans="1:3">
+    <row r="243" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A243" s="1" t="s">
         <v>508</v>
       </c>
@@ -5010,7 +5023,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="244" spans="1:3">
+    <row r="244" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A244" s="1" t="s">
         <v>508</v>
       </c>
@@ -5021,7 +5034,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="245" spans="1:3">
+    <row r="245" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A245" s="1" t="s">
         <v>508</v>
       </c>
@@ -5032,7 +5045,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="246" spans="1:3">
+    <row r="246" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A246" s="1" t="s">
         <v>508</v>
       </c>
@@ -5043,7 +5056,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="247" spans="1:3">
+    <row r="247" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A247" s="1" t="s">
         <v>508</v>
       </c>
@@ -5054,7 +5067,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="248" spans="1:3">
+    <row r="248" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A248" s="1" t="s">
         <v>508</v>
       </c>
@@ -5065,7 +5078,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="249" spans="1:3">
+    <row r="249" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A249" s="1" t="s">
         <v>508</v>
       </c>
@@ -5076,7 +5089,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="250" spans="1:3">
+    <row r="250" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A250" s="1" t="s">
         <v>508</v>
       </c>
@@ -5087,7 +5100,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="251" spans="1:3">
+    <row r="251" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A251" s="1" t="s">
         <v>508</v>
       </c>
@@ -5098,7 +5111,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="252" spans="1:3">
+    <row r="252" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A252" s="1" t="s">
         <v>508</v>
       </c>
@@ -5109,7 +5122,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="253" spans="1:3">
+    <row r="253" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A253" s="1" t="s">
         <v>508</v>
       </c>
@@ -5120,7 +5133,7 @@
         <v>522</v>
       </c>
     </row>
-    <row r="254" spans="1:3">
+    <row r="254" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A254" s="1" t="s">
         <v>508</v>
       </c>
@@ -5131,7 +5144,7 @@
         <v>537</v>
       </c>
     </row>
-    <row r="255" spans="1:3">
+    <row r="255" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A255" s="1" t="s">
         <v>508</v>
       </c>
@@ -5142,7 +5155,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="256" spans="1:3">
+    <row r="256" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A256" s="1" t="s">
         <v>508</v>
       </c>
@@ -5153,7 +5166,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="257" spans="1:3">
+    <row r="257" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A257" s="1" t="s">
         <v>508</v>
       </c>
@@ -5164,7 +5177,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="258" spans="1:3">
+    <row r="258" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A258" s="1" t="s">
         <v>508</v>
       </c>
@@ -5175,7 +5188,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="259" spans="1:3">
+    <row r="259" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A259" s="1" t="s">
         <v>508</v>
       </c>
@@ -5186,7 +5199,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="260" spans="1:3">
+    <row r="260" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A260" s="1" t="s">
         <v>508</v>
       </c>
@@ -5197,7 +5210,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="261" spans="1:3">
+    <row r="261" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A261" s="1" t="s">
         <v>508</v>
       </c>
@@ -5208,7 +5221,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="262" spans="1:3">
+    <row r="262" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A262" s="1" t="s">
         <v>508</v>
       </c>
@@ -5219,7 +5232,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="263" spans="1:3">
+    <row r="263" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A263" s="1" t="s">
         <v>508</v>
       </c>
@@ -5230,7 +5243,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="264" spans="1:3">
+    <row r="264" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A264" s="1" t="s">
         <v>509</v>
       </c>
@@ -5241,7 +5254,7 @@
         <v>522</v>
       </c>
     </row>
-    <row r="265" spans="1:3">
+    <row r="265" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A265" s="1" t="s">
         <v>508</v>
       </c>
@@ -5252,7 +5265,7 @@
         <v>529</v>
       </c>
     </row>
-    <row r="266" spans="1:3">
+    <row r="266" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A266" s="1" t="s">
         <v>508</v>
       </c>
@@ -5263,7 +5276,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="267" spans="1:3">
+    <row r="267" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A267" s="1" t="s">
         <v>508</v>
       </c>
@@ -5274,7 +5287,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="268" spans="1:3">
+    <row r="268" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A268" s="1" t="s">
         <v>508</v>
       </c>
@@ -5285,7 +5298,7 @@
         <v>539</v>
       </c>
     </row>
-    <row r="269" spans="1:3">
+    <row r="269" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A269" s="1" t="s">
         <v>508</v>
       </c>
@@ -5296,7 +5309,7 @@
         <v>538</v>
       </c>
     </row>
-    <row r="270" spans="1:3">
+    <row r="270" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A270" s="1" t="s">
         <v>508</v>
       </c>
@@ -5307,7 +5320,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="271" spans="1:3">
+    <row r="271" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A271" s="1" t="s">
         <v>508</v>
       </c>
@@ -5318,7 +5331,7 @@
         <v>534</v>
       </c>
     </row>
-    <row r="272" spans="1:3">
+    <row r="272" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A272" s="1" t="s">
         <v>508</v>
       </c>
@@ -5329,7 +5342,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="273" spans="1:3">
+    <row r="273" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A273" s="1" t="s">
         <v>508</v>
       </c>
@@ -5340,7 +5353,7 @@
         <v>533</v>
       </c>
     </row>
-    <row r="274" spans="1:3">
+    <row r="274" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A274" s="1" t="s">
         <v>508</v>
       </c>
@@ -5351,7 +5364,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="275" spans="1:3">
+    <row r="275" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A275" s="1" t="s">
         <v>509</v>
       </c>
@@ -5362,7 +5375,7 @@
         <v>540</v>
       </c>
     </row>
-    <row r="276" spans="1:3">
+    <row r="276" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A276" s="1" t="s">
         <v>508</v>
       </c>
@@ -5373,7 +5386,7 @@
         <v>525</v>
       </c>
     </row>
-    <row r="277" spans="1:3">
+    <row r="277" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A277" s="1" t="s">
         <v>508</v>
       </c>
@@ -5384,7 +5397,7 @@
         <v>539</v>
       </c>
     </row>
-    <row r="278" spans="1:3">
+    <row r="278" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A278" s="1" t="s">
         <v>508</v>
       </c>
@@ -5395,7 +5408,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="279" spans="1:3">
+    <row r="279" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A279" s="1" t="s">
         <v>508</v>
       </c>
@@ -5406,7 +5419,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="280" spans="1:3">
+    <row r="280" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A280" s="1" t="s">
         <v>508</v>
       </c>
@@ -5417,7 +5430,7 @@
         <v>521</v>
       </c>
     </row>
-    <row r="281" spans="1:3">
+    <row r="281" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A281" s="1" t="s">
         <v>508</v>
       </c>
@@ -5428,7 +5441,7 @@
         <v>521</v>
       </c>
     </row>
-    <row r="282" spans="1:3">
+    <row r="282" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A282" s="1" t="s">
         <v>508</v>
       </c>
@@ -5439,7 +5452,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="283" spans="1:3">
+    <row r="283" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A283" s="1" t="s">
         <v>508</v>
       </c>
@@ -5450,7 +5463,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="284" spans="1:3">
+    <row r="284" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A284" s="1" t="s">
         <v>508</v>
       </c>
@@ -5461,7 +5474,7 @@
         <v>521</v>
       </c>
     </row>
-    <row r="285" spans="1:3">
+    <row r="285" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A285" s="1" t="s">
         <v>508</v>
       </c>
@@ -5472,7 +5485,7 @@
         <v>534</v>
       </c>
     </row>
-    <row r="286" spans="1:3">
+    <row r="286" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A286" s="1" t="s">
         <v>508</v>
       </c>
@@ -5483,7 +5496,7 @@
         <v>521</v>
       </c>
     </row>
-    <row r="287" spans="1:3">
+    <row r="287" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A287" s="1" t="s">
         <v>508</v>
       </c>
@@ -5494,7 +5507,7 @@
         <v>534</v>
       </c>
     </row>
-    <row r="288" spans="1:3">
+    <row r="288" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A288" s="1" t="s">
         <v>508</v>
       </c>
@@ -5505,7 +5518,7 @@
         <v>541</v>
       </c>
     </row>
-    <row r="289" spans="1:3">
+    <row r="289" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A289" s="1" t="s">
         <v>508</v>
       </c>
@@ -5516,7 +5529,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="290" spans="1:3">
+    <row r="290" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A290" s="1" t="s">
         <v>508</v>
       </c>
@@ -5527,7 +5540,7 @@
         <v>542</v>
       </c>
     </row>
-    <row r="291" spans="1:3">
+    <row r="291" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A291" s="1" t="s">
         <v>509</v>
       </c>
@@ -5538,7 +5551,7 @@
         <v>539</v>
       </c>
     </row>
-    <row r="292" spans="1:3">
+    <row r="292" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A292" s="1" t="s">
         <v>508</v>
       </c>
@@ -5549,7 +5562,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="293" spans="1:3">
+    <row r="293" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A293" s="1" t="s">
         <v>510</v>
       </c>
@@ -5560,7 +5573,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="294" spans="1:3">
+    <row r="294" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A294" s="1" t="s">
         <v>510</v>
       </c>
@@ -5571,7 +5584,7 @@
         <v>539</v>
       </c>
     </row>
-    <row r="295" spans="1:3">
+    <row r="295" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A295" s="1" t="s">
         <v>510</v>
       </c>
@@ -5582,7 +5595,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="296" spans="1:3">
+    <row r="296" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A296" s="1" t="s">
         <v>508</v>
       </c>
@@ -5593,7 +5606,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="297" spans="1:3">
+    <row r="297" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A297" s="1" t="s">
         <v>508</v>
       </c>
@@ -5604,7 +5617,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="298" spans="1:3">
+    <row r="298" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A298" s="1" t="s">
         <v>508</v>
       </c>
@@ -5615,7 +5628,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="299" spans="1:3">
+    <row r="299" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A299" s="1" t="s">
         <v>508</v>
       </c>
@@ -5626,7 +5639,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="300" spans="1:3">
+    <row r="300" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A300" s="1" t="s">
         <v>508</v>
       </c>
@@ -5637,7 +5650,7 @@
         <v>539</v>
       </c>
     </row>
-    <row r="301" spans="1:3">
+    <row r="301" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A301" s="1" t="s">
         <v>508</v>
       </c>
@@ -5648,7 +5661,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="302" spans="1:3">
+    <row r="302" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A302" s="1" t="s">
         <v>508</v>
       </c>
@@ -5659,7 +5672,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="303" spans="1:3">
+    <row r="303" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A303" s="1" t="s">
         <v>508</v>
       </c>
@@ -5670,7 +5683,7 @@
         <v>521</v>
       </c>
     </row>
-    <row r="304" spans="1:3">
+    <row r="304" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A304" s="1" t="s">
         <v>509</v>
       </c>
@@ -5681,7 +5694,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="305" spans="1:3">
+    <row r="305" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A305" s="1" t="s">
         <v>508</v>
       </c>
@@ -5692,7 +5705,7 @@
         <v>543</v>
       </c>
     </row>
-    <row r="306" spans="1:3">
+    <row r="306" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A306" s="1" t="s">
         <v>508</v>
       </c>
@@ -5703,7 +5716,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="307" spans="1:3">
+    <row r="307" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A307" s="1" t="s">
         <v>508</v>
       </c>
@@ -5714,7 +5727,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="308" spans="1:3">
+    <row r="308" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A308" s="1" t="s">
         <v>508</v>
       </c>
@@ -5725,7 +5738,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="309" spans="1:3">
+    <row r="309" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A309" s="1" t="s">
         <v>509</v>
       </c>
@@ -5736,7 +5749,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="310" spans="1:3">
+    <row r="310" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A310" s="1" t="s">
         <v>508</v>
       </c>
@@ -5747,7 +5760,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="311" spans="1:3">
+    <row r="311" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A311" s="1" t="s">
         <v>508</v>
       </c>
@@ -5758,7 +5771,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="312" spans="1:3">
+    <row r="312" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A312" s="1" t="s">
         <v>508</v>
       </c>
@@ -5769,7 +5782,7 @@
         <v>539</v>
       </c>
     </row>
-    <row r="313" spans="1:3">
+    <row r="313" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A313" s="1" t="s">
         <v>508</v>
       </c>
@@ -5780,7 +5793,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="314" spans="1:3">
+    <row r="314" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A314" s="1" t="s">
         <v>508</v>
       </c>
@@ -5791,7 +5804,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="315" spans="1:3">
+    <row r="315" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A315" s="1" t="s">
         <v>508</v>
       </c>
@@ -5802,7 +5815,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="316" spans="1:3">
+    <row r="316" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A316" s="1" t="s">
         <v>508</v>
       </c>
@@ -5813,7 +5826,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="317" spans="1:3">
+    <row r="317" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A317" s="1" t="s">
         <v>508</v>
       </c>
@@ -5824,7 +5837,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="318" spans="1:3">
+    <row r="318" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A318" s="1" t="s">
         <v>508</v>
       </c>
@@ -5835,7 +5848,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="319" spans="1:3">
+    <row r="319" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A319" s="1" t="s">
         <v>508</v>
       </c>
@@ -5846,7 +5859,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="320" spans="1:3">
+    <row r="320" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A320" s="1" t="s">
         <v>508</v>
       </c>
@@ -5857,7 +5870,7 @@
         <v>521</v>
       </c>
     </row>
-    <row r="321" spans="1:3">
+    <row r="321" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A321" s="1" t="s">
         <v>508</v>
       </c>
@@ -5868,7 +5881,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="322" spans="1:3">
+    <row r="322" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A322" s="1" t="s">
         <v>508</v>
       </c>
@@ -5879,7 +5892,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="323" spans="1:3">
+    <row r="323" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A323" s="1" t="s">
         <v>508</v>
       </c>
@@ -5890,7 +5903,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="324" spans="1:3">
+    <row r="324" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A324" s="1" t="s">
         <v>508</v>
       </c>
@@ -5901,7 +5914,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="325" spans="1:3">
+    <row r="325" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A325" s="1" t="s">
         <v>508</v>
       </c>
@@ -5912,7 +5925,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="326" spans="1:3">
+    <row r="326" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A326" s="1" t="s">
         <v>508</v>
       </c>
@@ -5923,7 +5936,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="327" spans="1:3">
+    <row r="327" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A327" s="1" t="s">
         <v>508</v>
       </c>
@@ -5934,7 +5947,7 @@
         <v>529</v>
       </c>
     </row>
-    <row r="328" spans="1:3">
+    <row r="328" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A328" s="1" t="s">
         <v>508</v>
       </c>
@@ -5945,7 +5958,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="329" spans="1:3">
+    <row r="329" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A329" s="1" t="s">
         <v>510</v>
       </c>
@@ -5956,7 +5969,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="330" spans="1:3">
+    <row r="330" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A330" s="1"/>
       <c r="B330" s="2" t="s">
         <v>34</v>
@@ -5965,7 +5978,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="331" spans="1:3">
+    <row r="331" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A331" s="1" t="s">
         <v>508</v>
       </c>
@@ -5976,7 +5989,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="332" spans="1:3">
+    <row r="332" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A332" s="1" t="s">
         <v>508</v>
       </c>
@@ -5987,7 +6000,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="333" spans="1:3">
+    <row r="333" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A333" s="1" t="s">
         <v>508</v>
       </c>
@@ -5998,7 +6011,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="334" spans="1:3">
+    <row r="334" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A334" s="1" t="s">
         <v>508</v>
       </c>
@@ -6009,7 +6022,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="335" spans="1:3">
+    <row r="335" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A335" s="1" t="s">
         <v>508</v>
       </c>
@@ -6020,7 +6033,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="336" spans="1:3">
+    <row r="336" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A336" s="1" t="s">
         <v>508</v>
       </c>
@@ -6031,7 +6044,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="337" spans="1:3">
+    <row r="337" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A337" s="1" t="s">
         <v>508</v>
       </c>
@@ -6042,7 +6055,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="338" spans="1:3">
+    <row r="338" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A338" s="1" t="s">
         <v>508</v>
       </c>
@@ -6053,7 +6066,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="339" spans="1:3">
+    <row r="339" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A339" s="1" t="s">
         <v>508</v>
       </c>
@@ -6064,7 +6077,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="340" spans="1:3">
+    <row r="340" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A340" s="1" t="s">
         <v>508</v>
       </c>
@@ -6075,7 +6088,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="341" spans="1:3">
+    <row r="341" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A341" s="1" t="s">
         <v>508</v>
       </c>
@@ -6086,7 +6099,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="342" spans="1:3">
+    <row r="342" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A342" s="1" t="s">
         <v>508</v>
       </c>
@@ -6097,7 +6110,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="343" spans="1:3">
+    <row r="343" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A343" s="1" t="s">
         <v>508</v>
       </c>
@@ -6108,7 +6121,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="344" spans="1:3">
+    <row r="344" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A344" s="1" t="s">
         <v>508</v>
       </c>
@@ -6119,7 +6132,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="345" spans="1:3">
+    <row r="345" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A345" s="1" t="s">
         <v>508</v>
       </c>
@@ -6130,7 +6143,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="346" spans="1:3">
+    <row r="346" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A346" s="1" t="s">
         <v>508</v>
       </c>
@@ -6141,7 +6154,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="347" spans="1:3">
+    <row r="347" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A347" s="1" t="s">
         <v>508</v>
       </c>
@@ -6152,7 +6165,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="348" spans="1:3">
+    <row r="348" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A348" s="1" t="s">
         <v>508</v>
       </c>
@@ -6163,7 +6176,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="349" spans="1:3">
+    <row r="349" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A349" s="1" t="s">
         <v>508</v>
       </c>
@@ -6174,7 +6187,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="350" spans="1:3">
+    <row r="350" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A350" s="1" t="s">
         <v>508</v>
       </c>
@@ -6185,7 +6198,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="351" spans="1:3">
+    <row r="351" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A351" s="1" t="s">
         <v>508</v>
       </c>
@@ -6196,7 +6209,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="352" spans="1:3">
+    <row r="352" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A352" s="1" t="s">
         <v>508</v>
       </c>
@@ -6207,7 +6220,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="353" spans="1:3">
+    <row r="353" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A353" s="1" t="s">
         <v>508</v>
       </c>
@@ -6218,7 +6231,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="354" spans="1:3">
+    <row r="354" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A354" s="1" t="s">
         <v>508</v>
       </c>
@@ -6229,7 +6242,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="355" spans="1:3">
+    <row r="355" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A355" s="1" t="s">
         <v>508</v>
       </c>
@@ -6240,7 +6253,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="356" spans="1:3">
+    <row r="356" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A356" s="1" t="s">
         <v>508</v>
       </c>
@@ -6251,7 +6264,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="357" spans="1:3">
+    <row r="357" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A357" s="1" t="s">
         <v>508</v>
       </c>
@@ -6262,7 +6275,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="358" spans="1:3">
+    <row r="358" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A358" s="1" t="s">
         <v>508</v>
       </c>
@@ -6273,7 +6286,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="359" spans="1:3">
+    <row r="359" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A359" s="1" t="s">
         <v>508</v>
       </c>
@@ -6284,7 +6297,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="360" spans="1:3">
+    <row r="360" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A360" s="1" t="s">
         <v>508</v>
       </c>
@@ -6295,7 +6308,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="361" spans="1:3">
+    <row r="361" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A361" s="1" t="s">
         <v>508</v>
       </c>
@@ -6306,7 +6319,7 @@
         <v>539</v>
       </c>
     </row>
-    <row r="362" spans="1:3">
+    <row r="362" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A362" s="1" t="s">
         <v>508</v>
       </c>
@@ -6317,7 +6330,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="363" spans="1:3">
+    <row r="363" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A363" s="1" t="s">
         <v>508</v>
       </c>
@@ -6328,7 +6341,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="364" spans="1:3">
+    <row r="364" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A364" s="1" t="s">
         <v>510</v>
       </c>
@@ -6339,7 +6352,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="365" spans="1:3">
+    <row r="365" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A365" s="1" t="s">
         <v>508</v>
       </c>
@@ -6350,7 +6363,7 @@
         <v>539</v>
       </c>
     </row>
-    <row r="366" spans="1:3">
+    <row r="366" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A366" s="1" t="s">
         <v>509</v>
       </c>
@@ -6361,7 +6374,7 @@
         <v>539</v>
       </c>
     </row>
-    <row r="367" spans="1:3">
+    <row r="367" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A367" s="1" t="s">
         <v>508</v>
       </c>
@@ -6372,7 +6385,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="368" spans="1:3">
+    <row r="368" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A368" s="1" t="s">
         <v>508</v>
       </c>
@@ -6383,7 +6396,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="369" spans="1:3">
+    <row r="369" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A369" s="1" t="s">
         <v>508</v>
       </c>
@@ -6394,7 +6407,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="370" spans="1:3">
+    <row r="370" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A370" s="1" t="s">
         <v>508</v>
       </c>
@@ -6405,7 +6418,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="371" spans="1:3">
+    <row r="371" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A371" s="1"/>
       <c r="B371" s="2" t="s">
         <v>476</v>
@@ -6414,7 +6427,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="372" spans="1:3">
+    <row r="372" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A372" s="1" t="s">
         <v>509</v>
       </c>
@@ -6425,7 +6438,7 @@
         <v>544</v>
       </c>
     </row>
-    <row r="373" spans="1:3">
+    <row r="373" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A373" s="1" t="s">
         <v>508</v>
       </c>
@@ -6436,7 +6449,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="374" spans="1:3">
+    <row r="374" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A374" s="1" t="s">
         <v>508</v>
       </c>
@@ -6447,7 +6460,7 @@
         <v>545</v>
       </c>
     </row>
-    <row r="375" spans="1:3">
+    <row r="375" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A375" s="1" t="s">
         <v>510</v>
       </c>
@@ -6458,7 +6471,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="376" spans="1:3">
+    <row r="376" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A376" s="1" t="s">
         <v>508</v>
       </c>
@@ -6469,7 +6482,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="377" spans="1:3">
+    <row r="377" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A377" s="1" t="s">
         <v>508</v>
       </c>
@@ -6480,7 +6493,7 @@
         <v>546</v>
       </c>
     </row>
-    <row r="378" spans="1:3">
+    <row r="378" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A378" s="1" t="s">
         <v>508</v>
       </c>
@@ -6491,7 +6504,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="379" spans="1:3">
+    <row r="379" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A379" s="1" t="s">
         <v>508</v>
       </c>
@@ -6502,7 +6515,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="380" spans="1:3">
+    <row r="380" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A380" s="1" t="s">
         <v>509</v>
       </c>
@@ -6513,7 +6526,7 @@
         <v>528</v>
       </c>
     </row>
-    <row r="381" spans="1:3">
+    <row r="381" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A381" s="1" t="s">
         <v>510</v>
       </c>
@@ -6524,7 +6537,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="382" spans="1:3">
+    <row r="382" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A382" s="1" t="s">
         <v>510</v>
       </c>
@@ -6535,7 +6548,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="383" spans="1:3">
+    <row r="383" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A383" s="1" t="s">
         <v>510</v>
       </c>
@@ -6546,7 +6559,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="384" spans="1:3">
+    <row r="384" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A384" s="1" t="s">
         <v>510</v>
       </c>
@@ -6557,7 +6570,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="385" spans="1:3">
+    <row r="385" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A385" s="1" t="s">
         <v>510</v>
       </c>
@@ -6568,7 +6581,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="386" spans="1:3">
+    <row r="386" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A386" s="1" t="s">
         <v>510</v>
       </c>
@@ -6579,7 +6592,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="387" spans="1:3">
+    <row r="387" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A387" s="1" t="s">
         <v>508</v>
       </c>
@@ -6590,7 +6603,7 @@
         <v>539</v>
       </c>
     </row>
-    <row r="388" spans="1:3">
+    <row r="388" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A388" s="1" t="s">
         <v>508</v>
       </c>
@@ -6601,7 +6614,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="389" spans="1:3">
+    <row r="389" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A389" s="1" t="s">
         <v>508</v>
       </c>
@@ -6612,7 +6625,7 @@
         <v>521</v>
       </c>
     </row>
-    <row r="390" spans="1:3">
+    <row r="390" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A390" s="1" t="s">
         <v>508</v>
       </c>
@@ -6623,7 +6636,7 @@
         <v>529</v>
       </c>
     </row>
-    <row r="391" spans="1:3">
+    <row r="391" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A391" s="1" t="s">
         <v>508</v>
       </c>
@@ -6634,7 +6647,7 @@
         <v>521</v>
       </c>
     </row>
-    <row r="392" spans="1:3">
+    <row r="392" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A392" s="1" t="s">
         <v>508</v>
       </c>
@@ -6645,7 +6658,7 @@
         <v>544</v>
       </c>
     </row>
-    <row r="393" spans="1:3">
+    <row r="393" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A393" s="1" t="s">
         <v>508</v>
       </c>
@@ -6656,7 +6669,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="394" spans="1:3">
+    <row r="394" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A394" s="1" t="s">
         <v>508</v>
       </c>
@@ -6667,7 +6680,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="395" spans="1:3">
+    <row r="395" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A395" s="1" t="s">
         <v>508</v>
       </c>
@@ -6678,7 +6691,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="396" spans="1:3">
+    <row r="396" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A396" s="1" t="s">
         <v>508</v>
       </c>
@@ -6689,7 +6702,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="397" spans="1:3">
+    <row r="397" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A397" s="1" t="s">
         <v>508</v>
       </c>
@@ -6700,7 +6713,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="398" spans="1:3">
+    <row r="398" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A398" s="1" t="s">
         <v>508</v>
       </c>
@@ -6711,7 +6724,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="399" spans="1:3">
+    <row r="399" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A399" s="1" t="s">
         <v>508</v>
       </c>
@@ -6722,7 +6735,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="400" spans="1:3">
+    <row r="400" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A400" s="1" t="s">
         <v>508</v>
       </c>
@@ -6733,7 +6746,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="401" spans="1:3">
+    <row r="401" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A401" s="1" t="s">
         <v>509</v>
       </c>
@@ -6744,7 +6757,7 @@
         <v>547</v>
       </c>
     </row>
-    <row r="402" spans="1:3">
+    <row r="402" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A402" s="1"/>
       <c r="B402" s="2" t="s">
         <v>278</v>
@@ -6753,7 +6766,7 @@
         <v>528</v>
       </c>
     </row>
-    <row r="403" spans="1:3">
+    <row r="403" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A403" s="1" t="s">
         <v>508</v>
       </c>
@@ -6764,7 +6777,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="404" spans="1:3">
+    <row r="404" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A404" s="1" t="s">
         <v>508</v>
       </c>
@@ -6775,7 +6788,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="405" spans="1:3">
+    <row r="405" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A405" s="1" t="s">
         <v>508</v>
       </c>
@@ -6786,7 +6799,7 @@
         <v>521</v>
       </c>
     </row>
-    <row r="406" spans="1:3">
+    <row r="406" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A406" s="1" t="s">
         <v>508</v>
       </c>
@@ -6797,7 +6810,7 @@
         <v>541</v>
       </c>
     </row>
-    <row r="407" spans="1:3">
+    <row r="407" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A407" s="1" t="s">
         <v>509</v>
       </c>
@@ -6808,7 +6821,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="408" spans="1:3">
+    <row r="408" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A408" s="1" t="s">
         <v>508</v>
       </c>
@@ -6819,7 +6832,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="409" spans="1:3">
+    <row r="409" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A409" s="1" t="s">
         <v>508</v>
       </c>
@@ -6830,7 +6843,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="410" spans="1:3">
+    <row r="410" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A410" s="1" t="s">
         <v>508</v>
       </c>
@@ -6841,7 +6854,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="411" spans="1:3">
+    <row r="411" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A411" s="1" t="s">
         <v>508</v>
       </c>
@@ -6852,7 +6865,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="412" spans="1:3">
+    <row r="412" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A412" s="1" t="s">
         <v>508</v>
       </c>
@@ -6863,7 +6876,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="413" spans="1:3">
+    <row r="413" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A413" s="1" t="s">
         <v>508</v>
       </c>
@@ -6874,7 +6887,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="414" spans="1:3">
+    <row r="414" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A414" s="1" t="s">
         <v>508</v>
       </c>
@@ -6885,7 +6898,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="415" spans="1:3">
+    <row r="415" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A415" s="1" t="s">
         <v>508</v>
       </c>
@@ -6896,7 +6909,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="416" spans="1:3">
+    <row r="416" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A416" s="1" t="s">
         <v>508</v>
       </c>
@@ -6907,7 +6920,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="417" spans="1:3">
+    <row r="417" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A417" s="1" t="s">
         <v>508</v>
       </c>
@@ -6918,7 +6931,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="418" spans="1:3">
+    <row r="418" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A418" s="1" t="s">
         <v>508</v>
       </c>
@@ -6929,7 +6942,7 @@
         <v>529</v>
       </c>
     </row>
-    <row r="419" spans="1:3">
+    <row r="419" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A419" s="1" t="s">
         <v>508</v>
       </c>
@@ -6940,7 +6953,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="420" spans="1:3">
+    <row r="420" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A420" s="1" t="s">
         <v>509</v>
       </c>
@@ -6951,7 +6964,7 @@
         <v>539</v>
       </c>
     </row>
-    <row r="421" spans="1:3">
+    <row r="421" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A421" s="1" t="s">
         <v>508</v>
       </c>
@@ -6962,7 +6975,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="422" spans="1:3">
+    <row r="422" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A422" s="1" t="s">
         <v>508</v>
       </c>
@@ -6973,7 +6986,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="423" spans="1:3">
+    <row r="423" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A423" s="1" t="s">
         <v>508</v>
       </c>
@@ -6984,7 +6997,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="424" spans="1:3">
+    <row r="424" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A424" s="1" t="s">
         <v>508</v>
       </c>
@@ -6995,7 +7008,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="425" spans="1:3">
+    <row r="425" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A425" s="1" t="s">
         <v>508</v>
       </c>
@@ -7006,7 +7019,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="426" spans="1:3">
+    <row r="426" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A426" s="1" t="s">
         <v>508</v>
       </c>
@@ -7017,7 +7030,7 @@
         <v>541</v>
       </c>
     </row>
-    <row r="427" spans="1:3">
+    <row r="427" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A427" s="1" t="s">
         <v>508</v>
       </c>
@@ -7028,7 +7041,7 @@
         <v>529</v>
       </c>
     </row>
-    <row r="428" spans="1:3">
+    <row r="428" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A428" s="1" t="s">
         <v>508</v>
       </c>
@@ -7039,7 +7052,7 @@
         <v>548</v>
       </c>
     </row>
-    <row r="429" spans="1:3">
+    <row r="429" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A429" s="1" t="s">
         <v>508</v>
       </c>
@@ -7050,7 +7063,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="430" spans="1:3">
+    <row r="430" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A430" s="1" t="s">
         <v>508</v>
       </c>
@@ -7061,7 +7074,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="431" spans="1:3">
+    <row r="431" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A431" s="1" t="s">
         <v>508</v>
       </c>
@@ -7072,7 +7085,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="432" spans="1:3">
+    <row r="432" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A432" s="1" t="s">
         <v>509</v>
       </c>
@@ -7083,7 +7096,7 @@
         <v>541</v>
       </c>
     </row>
-    <row r="433" spans="1:3">
+    <row r="433" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A433" s="1" t="s">
         <v>508</v>
       </c>
@@ -7094,7 +7107,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="434" spans="1:3">
+    <row r="434" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A434" s="1" t="s">
         <v>508</v>
       </c>
@@ -7105,7 +7118,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="435" spans="1:3">
+    <row r="435" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A435" s="1" t="s">
         <v>508</v>
       </c>
@@ -7116,7 +7129,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="436" spans="1:3">
+    <row r="436" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A436" s="1" t="s">
         <v>508</v>
       </c>
@@ -7127,7 +7140,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="437" spans="1:3">
+    <row r="437" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A437" s="1" t="s">
         <v>508</v>
       </c>
@@ -7138,7 +7151,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="438" spans="1:3">
+    <row r="438" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A438" s="1" t="s">
         <v>508</v>
       </c>
@@ -7149,7 +7162,7 @@
         <v>521</v>
       </c>
     </row>
-    <row r="439" spans="1:3">
+    <row r="439" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A439" s="1" t="s">
         <v>508</v>
       </c>
@@ -7160,7 +7173,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="440" spans="1:3">
+    <row r="440" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A440" s="1" t="s">
         <v>508</v>
       </c>
@@ -7171,7 +7184,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="441" spans="1:3">
+    <row r="441" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A441" s="1" t="s">
         <v>508</v>
       </c>
@@ -7182,7 +7195,7 @@
         <v>545</v>
       </c>
     </row>
-    <row r="442" spans="1:3">
+    <row r="442" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A442" s="1" t="s">
         <v>508</v>
       </c>
@@ -7193,7 +7206,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="443" spans="1:3">
+    <row r="443" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A443" s="1" t="s">
         <v>508</v>
       </c>
@@ -7204,7 +7217,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="444" spans="1:3">
+    <row r="444" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A444" s="1" t="s">
         <v>508</v>
       </c>
@@ -7215,7 +7228,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="445" spans="1:3">
+    <row r="445" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A445" s="1" t="s">
         <v>508</v>
       </c>
@@ -7226,7 +7239,7 @@
         <v>529</v>
       </c>
     </row>
-    <row r="446" spans="1:3">
+    <row r="446" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A446" s="1"/>
       <c r="B446" s="2" t="s">
         <v>507</v>
@@ -7235,7 +7248,7 @@
         <v>549</v>
       </c>
     </row>
-    <row r="447" spans="1:3">
+    <row r="447" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A447" s="1" t="s">
         <v>508</v>
       </c>
@@ -7246,7 +7259,7 @@
         <v>550</v>
       </c>
     </row>
-    <row r="448" spans="1:3">
+    <row r="448" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A448" s="1"/>
       <c r="B448" s="2" t="s">
         <v>503</v>
@@ -7255,7 +7268,7 @@
         <v>552</v>
       </c>
     </row>
-    <row r="449" spans="1:3">
+    <row r="449" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A449" s="1" t="s">
         <v>509</v>
       </c>
@@ -7266,7 +7279,7 @@
         <v>544</v>
       </c>
     </row>
-    <row r="450" spans="1:3">
+    <row r="450" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A450" s="1" t="s">
         <v>508</v>
       </c>
@@ -7277,7 +7290,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="451" spans="1:3">
+    <row r="451" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A451" s="1" t="s">
         <v>508</v>
       </c>
@@ -7288,7 +7301,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="452" spans="1:3">
+    <row r="452" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A452" s="1" t="s">
         <v>508</v>
       </c>
@@ -7299,7 +7312,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="453" spans="1:3">
+    <row r="453" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A453" s="1" t="s">
         <v>508</v>
       </c>
@@ -7310,7 +7323,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="454" spans="1:3">
+    <row r="454" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A454" s="1" t="s">
         <v>508</v>
       </c>
@@ -7321,7 +7334,7 @@
         <v>553</v>
       </c>
     </row>
-    <row r="455" spans="1:3">
+    <row r="455" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A455" s="1"/>
       <c r="B455" s="2" t="s">
         <v>37</v>
@@ -7330,7 +7343,7 @@
         <v>539</v>
       </c>
     </row>
-    <row r="456" spans="1:3">
+    <row r="456" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A456" s="1" t="s">
         <v>508</v>
       </c>
@@ -7341,7 +7354,7 @@
         <v>541</v>
       </c>
     </row>
-    <row r="457" spans="1:3">
+    <row r="457" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A457" s="1" t="s">
         <v>508</v>
       </c>
@@ -7352,7 +7365,7 @@
         <v>521</v>
       </c>
     </row>
-    <row r="458" spans="1:3">
+    <row r="458" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A458" s="1" t="s">
         <v>508</v>
       </c>
@@ -7363,7 +7376,7 @@
         <v>539</v>
       </c>
     </row>
-    <row r="459" spans="1:3">
+    <row r="459" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A459" s="1" t="s">
         <v>508</v>
       </c>
@@ -7374,7 +7387,7 @@
         <v>539</v>
       </c>
     </row>
-    <row r="460" spans="1:3">
+    <row r="460" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A460" s="1" t="s">
         <v>508</v>
       </c>
@@ -7385,7 +7398,7 @@
         <v>539</v>
       </c>
     </row>
-    <row r="461" spans="1:3">
+    <row r="461" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A461" s="1"/>
       <c r="B461" s="2" t="s">
         <v>279</v>
@@ -7394,7 +7407,7 @@
         <v>543</v>
       </c>
     </row>
-    <row r="462" spans="1:3">
+    <row r="462" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A462" s="1" t="s">
         <v>508</v>
       </c>
@@ -7405,7 +7418,7 @@
         <v>529</v>
       </c>
     </row>
-    <row r="463" spans="1:3">
+    <row r="463" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A463" s="1" t="s">
         <v>508</v>
       </c>
@@ -7416,7 +7429,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="464" spans="1:3">
+    <row r="464" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A464" s="1" t="s">
         <v>508</v>
       </c>
@@ -7427,7 +7440,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="465" spans="1:3">
+    <row r="465" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A465" s="1" t="s">
         <v>508</v>
       </c>
@@ -7438,7 +7451,7 @@
         <v>550</v>
       </c>
     </row>
-    <row r="466" spans="1:3">
+    <row r="466" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A466" s="1" t="s">
         <v>509</v>
       </c>
@@ -7449,7 +7462,7 @@
         <v>545</v>
       </c>
     </row>
-    <row r="467" spans="1:3">
+    <row r="467" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A467" s="1" t="s">
         <v>508</v>
       </c>
@@ -7460,7 +7473,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="468" spans="1:3">
+    <row r="468" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A468" s="1" t="s">
         <v>508</v>
       </c>
@@ -7471,7 +7484,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="469" spans="1:3">
+    <row r="469" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A469" s="1" t="s">
         <v>508</v>
       </c>
@@ -7482,7 +7495,7 @@
         <v>539</v>
       </c>
     </row>
-    <row r="470" spans="1:3">
+    <row r="470" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A470" s="1" t="s">
         <v>508</v>
       </c>
@@ -7493,7 +7506,7 @@
         <v>554</v>
       </c>
     </row>
-    <row r="471" spans="1:3">
+    <row r="471" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A471" s="1" t="s">
         <v>508</v>
       </c>
@@ -7504,7 +7517,7 @@
         <v>521</v>
       </c>
     </row>
-    <row r="472" spans="1:3">
+    <row r="472" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A472" s="1" t="s">
         <v>508</v>
       </c>
@@ -7515,7 +7528,7 @@
         <v>521</v>
       </c>
     </row>
-    <row r="473" spans="1:3">
+    <row r="473" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A473" s="1" t="s">
         <v>509</v>
       </c>
@@ -7526,7 +7539,7 @@
         <v>521</v>
       </c>
     </row>
-    <row r="474" spans="1:3">
+    <row r="474" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A474" s="1" t="s">
         <v>508</v>
       </c>
@@ -7537,7 +7550,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="475" spans="1:3">
+    <row r="475" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A475" s="1" t="s">
         <v>508</v>
       </c>
@@ -7548,7 +7561,7 @@
         <v>550</v>
       </c>
     </row>
-    <row r="476" spans="1:3">
+    <row r="476" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A476" s="1" t="s">
         <v>508</v>
       </c>
@@ -7559,7 +7572,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="477" spans="1:3">
+    <row r="477" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A477" s="1" t="s">
         <v>509</v>
       </c>
@@ -7570,7 +7583,7 @@
         <v>532</v>
       </c>
     </row>
-    <row r="478" spans="1:3">
+    <row r="478" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A478" s="1" t="s">
         <v>509</v>
       </c>
@@ -7581,7 +7594,7 @@
         <v>539</v>
       </c>
     </row>
-    <row r="479" spans="1:3">
+    <row r="479" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A479" s="1" t="s">
         <v>509</v>
       </c>
@@ -7592,7 +7605,7 @@
         <v>539</v>
       </c>
     </row>
-    <row r="480" spans="1:3">
+    <row r="480" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A480" s="1" t="s">
         <v>509</v>
       </c>
@@ -7603,7 +7616,7 @@
         <v>544</v>
       </c>
     </row>
-    <row r="481" spans="1:3">
+    <row r="481" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A481" s="1" t="s">
         <v>509</v>
       </c>
@@ -7614,7 +7627,7 @@
         <v>539</v>
       </c>
     </row>
-    <row r="482" spans="1:3">
+    <row r="482" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A482" s="1" t="s">
         <v>508</v>
       </c>
@@ -7625,7 +7638,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="483" spans="1:3">
+    <row r="483" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A483" s="1" t="s">
         <v>508</v>
       </c>
@@ -7636,7 +7649,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="484" spans="1:3">
+    <row r="484" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A484" s="1" t="s">
         <v>508</v>
       </c>
@@ -7647,7 +7660,7 @@
         <v>530</v>
       </c>
     </row>
-    <row r="485" spans="1:3" ht="36">
+    <row r="485" spans="1:3" ht="37.5" x14ac:dyDescent="0.25">
       <c r="A485" s="1" t="s">
         <v>508</v>
       </c>
@@ -7658,7 +7671,7 @@
         <v>555</v>
       </c>
     </row>
-    <row r="486" spans="1:3">
+    <row r="486" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A486" s="1" t="s">
         <v>509</v>
       </c>
@@ -7669,7 +7682,7 @@
         <v>539</v>
       </c>
     </row>
-    <row r="487" spans="1:3">
+    <row r="487" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A487" s="1" t="s">
         <v>509</v>
       </c>
@@ -7680,7 +7693,7 @@
         <v>539</v>
       </c>
     </row>
-    <row r="488" spans="1:3">
+    <row r="488" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A488" s="1" t="s">
         <v>508</v>
       </c>
@@ -7691,7 +7704,7 @@
         <v>539</v>
       </c>
     </row>
-    <row r="489" spans="1:3" ht="36">
+    <row r="489" spans="1:3" ht="37.5" x14ac:dyDescent="0.25">
       <c r="A489" s="1" t="s">
         <v>510</v>
       </c>
@@ -7702,7 +7715,7 @@
         <v>555</v>
       </c>
     </row>
-    <row r="490" spans="1:3">
+    <row r="490" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A490" s="1" t="s">
         <v>508</v>
       </c>
@@ -7713,7 +7726,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="491" spans="1:3">
+    <row r="491" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A491" s="1" t="s">
         <v>508</v>
       </c>
@@ -7724,7 +7737,7 @@
         <v>521</v>
       </c>
     </row>
-    <row r="492" spans="1:3">
+    <row r="492" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A492" s="1" t="s">
         <v>508</v>
       </c>
@@ -7735,7 +7748,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="493" spans="1:3">
+    <row r="493" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A493" s="1" t="s">
         <v>508</v>
       </c>
@@ -7746,7 +7759,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="494" spans="1:3">
+    <row r="494" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A494" s="1" t="s">
         <v>508</v>
       </c>
@@ -7757,7 +7770,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="495" spans="1:3">
+    <row r="495" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A495" s="1" t="s">
         <v>508</v>
       </c>
@@ -7768,7 +7781,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="496" spans="1:3">
+    <row r="496" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A496" s="1" t="s">
         <v>508</v>
       </c>
@@ -7779,7 +7792,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="497" spans="1:3">
+    <row r="497" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A497" s="1" t="s">
         <v>508</v>
       </c>
@@ -7790,7 +7803,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="498" spans="1:3">
+    <row r="498" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A498" s="1" t="s">
         <v>508</v>
       </c>
@@ -7801,7 +7814,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="499" spans="1:3">
+    <row r="499" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A499" s="1" t="s">
         <v>508</v>
       </c>
@@ -7812,7 +7825,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="500" spans="1:3">
+    <row r="500" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A500" s="1" t="s">
         <v>508</v>
       </c>
@@ -7823,7 +7836,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="501" spans="1:3">
+    <row r="501" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A501" s="1" t="s">
         <v>508</v>
       </c>
@@ -7834,7 +7847,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="502" spans="1:3">
+    <row r="502" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A502" s="1"/>
       <c r="B502" s="2" t="s">
         <v>99</v>
@@ -7843,7 +7856,7 @@
         <v>539</v>
       </c>
     </row>
-    <row r="503" spans="1:3">
+    <row r="503" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A503" s="1" t="s">
         <v>508</v>
       </c>
@@ -7854,7 +7867,7 @@
         <v>521</v>
       </c>
     </row>
-    <row r="504" spans="1:3">
+    <row r="504" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A504" s="1" t="s">
         <v>508</v>
       </c>
@@ -7865,7 +7878,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="505" spans="1:3">
+    <row r="505" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A505" s="1" t="s">
         <v>508</v>
       </c>
@@ -7876,7 +7889,7 @@
         <v>541</v>
       </c>
     </row>
-    <row r="506" spans="1:3">
+    <row r="506" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A506" s="1" t="s">
         <v>508</v>
       </c>
@@ -7887,7 +7900,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="507" spans="1:3">
+    <row r="507" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A507" s="1" t="s">
         <v>508</v>
       </c>
@@ -7898,7 +7911,7 @@
         <v>547</v>
       </c>
     </row>
-    <row r="508" spans="1:3">
+    <row r="508" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A508" s="1" t="s">
         <v>509</v>
       </c>
@@ -7909,7 +7922,7 @@
         <v>539</v>
       </c>
     </row>
-    <row r="509" spans="1:3">
+    <row r="509" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A509" s="1" t="s">
         <v>508</v>
       </c>
@@ -7920,7 +7933,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="510" spans="1:3">
+    <row r="510" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A510" s="1" t="s">
         <v>508</v>
       </c>
@@ -7931,7 +7944,7 @@
         <v>530</v>
       </c>
     </row>
-    <row r="511" spans="1:3">
+    <row r="511" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A511" s="1" t="s">
         <v>508</v>
       </c>
@@ -7942,7 +7955,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="512" spans="1:3">
+    <row r="512" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A512" s="1" t="s">
         <v>508</v>
       </c>
@@ -7953,7 +7966,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="513" spans="1:3">
+    <row r="513" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A513" s="1" t="s">
         <v>508</v>
       </c>
@@ -7964,7 +7977,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="514" spans="1:3">
+    <row r="514" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A514" s="1" t="s">
         <v>508</v>
       </c>
@@ -7975,7 +7988,7 @@
         <v>538</v>
       </c>
     </row>
-    <row r="515" spans="1:3">
+    <row r="515" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A515" s="1" t="s">
         <v>508</v>
       </c>
@@ -7986,7 +7999,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="516" spans="1:3">
+    <row r="516" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A516" s="1" t="s">
         <v>508</v>
       </c>
@@ -7997,7 +8010,7 @@
         <v>556</v>
       </c>
     </row>
-    <row r="517" spans="1:3">
+    <row r="517" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A517" s="1" t="s">
         <v>508</v>
       </c>
@@ -8008,7 +8021,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="518" spans="1:3">
+    <row r="518" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A518" s="1" t="s">
         <v>508</v>
       </c>
@@ -8019,7 +8032,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="519" spans="1:3">
+    <row r="519" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A519" s="1" t="s">
         <v>508</v>
       </c>
@@ -8030,7 +8043,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="520" spans="1:3">
+    <row r="520" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A520" s="1" t="s">
         <v>508</v>
       </c>
@@ -8041,7 +8054,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="521" spans="1:3">
+    <row r="521" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A521" s="1" t="s">
         <v>508</v>
       </c>
@@ -8052,7 +8065,7 @@
         <v>529</v>
       </c>
     </row>
-    <row r="522" spans="1:3">
+    <row r="522" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A522" s="1" t="s">
         <v>508</v>
       </c>
@@ -8063,7 +8076,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="523" spans="1:3">
+    <row r="523" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A523" s="1" t="s">
         <v>509</v>
       </c>
@@ -8074,7 +8087,7 @@
         <v>547</v>
       </c>
     </row>
-    <row r="524" spans="1:3">
+    <row r="524" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A524" s="1" t="s">
         <v>508</v>
       </c>

</xml_diff>